<commit_message>
The 'TAWA_CustomerRequirements'document has been modified
</commit_message>
<xml_diff>
--- a/TAWA_CustomerRequirements.xlsx
+++ b/TAWA_CustomerRequirements.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nesma Files\ITI\SW Project Management\Travel-Adviser-Web-Application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\project management\project\Travel-Adviser-Web-Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8805"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -665,18 +665,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:T4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="187.85546875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="18.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="187.88671875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -700,7 +700,7 @@
       <c r="S1" s="14"/>
       <c r="T1" s="15"/>
     </row>
-    <row r="2" spans="1:21" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -724,7 +724,7 @@
       <c r="S2" s="14"/>
       <c r="T2" s="15"/>
     </row>
-    <row r="3" spans="1:21" ht="107.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
@@ -748,7 +748,7 @@
       <c r="S3" s="14"/>
       <c r="T3" s="15"/>
     </row>
-    <row r="4" spans="1:21" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
@@ -772,7 +772,7 @@
       <c r="S4" s="17"/>
       <c r="T4" s="18"/>
     </row>
-    <row r="5" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -799,7 +799,7 @@
       <c r="T5" s="8"/>
       <c r="U5" s="8"/>
     </row>
-    <row r="6" spans="1:21" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -812,7 +812,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:21" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
@@ -825,7 +825,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:21" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -838,7 +838,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:21" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
@@ -851,7 +851,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:21" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
@@ -864,7 +864,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:21" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="3"/>
@@ -873,47 +873,47 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:21" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:21" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:21" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:21" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:21" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:2" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:2" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
     </row>

</xml_diff>